<commit_message>
program runs on FLIP & reflection drafted with flowchart & initial tests
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryandirezze/Documents/GitHub/cs162_project1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044C07CF-4F79-2C48-8711-912DDDF48DE2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42E692F-98D2-A247-A52B-31FB0C4909FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="3620" windowWidth="13560" windowHeight="9740" xr2:uid="{4D30CEE1-22F0-F142-94D7-8797B0C7E02D}"/>
+    <workbookView xWindow="14620" yWindow="600" windowWidth="13380" windowHeight="12100" xr2:uid="{4D30CEE1-22F0-F142-94D7-8797B0C7E02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Test Case</t>
   </si>
@@ -182,13 +182,46 @@
     <t>Print a confirmation that the ant will not start in a random location, ask for board parameters, ask for ant's starting position, and initialize the ant on the board at the user specified location</t>
   </si>
   <si>
-    <t>Prompts menu selection after program completes</t>
-  </si>
-  <si>
-    <t>Board parameters input validation (very small &amp; large, and floats)</t>
-  </si>
-  <si>
-    <t>(User specified) Ant coordinates input validation (floats and on board's border)</t>
+    <t>Board parameters input validation (very small)</t>
+  </si>
+  <si>
+    <t>Board parameters input validation (very large)</t>
+  </si>
+  <si>
+    <t>Board parameters input validation (floats)</t>
+  </si>
+  <si>
+    <t>(User specified) Ant coordinates input validation (floats)</t>
+  </si>
+  <si>
+    <t>(User specified) Ant coordinates input validation (on board's border)</t>
+  </si>
+  <si>
+    <t>Input = 1</t>
+  </si>
+  <si>
+    <t>Input = 1,000</t>
+  </si>
+  <si>
+    <t>0 &lt; Input &lt; 1</t>
+  </si>
+  <si>
+    <t>Input = 0;
+Input = Columns/Rows</t>
+  </si>
+  <si>
+    <t>Board board = Board(rows, columns);
+rows/columns = input</t>
+  </si>
+  <si>
+    <t>Ant ant = Ant(rand_x, rand_y, board);
+rand_x, rand_y = input</t>
+  </si>
+  <si>
+    <t>Board prints and program executes as expected</t>
+  </si>
+  <si>
+    <t>Program crashes</t>
   </si>
 </sst>
 </file>
@@ -249,6 +282,21 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -267,21 +315,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -296,8 +329,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91E0D28D-2FAF-BA41-BD46-B0885AC20B2E}" name="Table1" displayName="Table1" ref="A1:E24" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:E24" xr:uid="{9CEE31C4-537E-784E-B735-C34D597D2EA1}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91E0D28D-2FAF-BA41-BD46-B0885AC20B2E}" name="Table1" displayName="Table1" ref="A1:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E26" xr:uid="{9CEE31C4-537E-784E-B735-C34D597D2EA1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -305,11 +338,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{746E146B-0052-854D-908B-92029FDFB4AB}" name="Test Case" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{EE6242AD-F31F-EC43-B235-0A67A7FBC4DE}" name="Input Values" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{06D4B865-992A-4848-B504-3BE4793F5AA1}" name="Driver Functions" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{72DF2831-A6C8-0C47-A4B5-AECB4AA2CFAF}" name="Expected Outcomes" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{30EFC03E-F14F-C64C-A45D-4A0955280E5F}" name="Observed Outcomes" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{746E146B-0052-854D-908B-92029FDFB4AB}" name="Test Case" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{EE6242AD-F31F-EC43-B235-0A67A7FBC4DE}" name="Input Values" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{06D4B865-992A-4848-B504-3BE4793F5AA1}" name="Driver Functions" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{72DF2831-A6C8-0C47-A4B5-AECB4AA2CFAF}" name="Expected Outcomes" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{30EFC03E-F14F-C64C-A45D-4A0955280E5F}" name="Observed Outcomes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -612,17 +645,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04431965-2B41-9E49-B5B7-8625799C189D}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="2"/>
@@ -925,19 +958,74 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="85">
+    <row r="22" spans="1:4" ht="68">
       <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="68">
+      <c r="A23" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="85">
-      <c r="A23" s="2" t="s">
-        <v>50</v>
+      <c r="B23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="68">
       <c r="A24" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="68">
+      <c r="A25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="85">
+      <c r="A26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>